<commit_message>
Added Feature to create new sheets that populate with a copy of data from previous weeks sheet;
</commit_message>
<xml_diff>
--- a/HTTP Request/Schedule/Dummy QC Schedule Copy.xlsx
+++ b/HTTP Request/Schedule/Dummy QC Schedule Copy.xlsx
@@ -5,12 +5,12 @@
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Documents\UiPath\HTTP Request\Schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Documents\UiPath\P3-schedulerassistant\HTTP Request\Schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02573D78-0F0E-400E-9B71-3A21E3FB7BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83A57A8-E3F1-4408-B288-46139689D7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="605" firstSheet="0" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="605" firstSheet="0" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Scheduling Rules" sheetId="77" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <x:sheet name="Trainer Info &amp; Skillsets" sheetId="1" r:id="rId3"/>
     <x:sheet name="QC Strategy" sheetId="2" state="hidden" r:id="rId4"/>
     <x:sheet name="QC-Groups" sheetId="3" state="hidden" r:id="rId5"/>
-    <x:sheet name="Dummy Schedule - Dec 6" sheetId="75" r:id="rId6"/>
-    <x:sheet name="Dec  13" sheetId="14" r:id="rId7"/>
+    <x:sheet name="12-6-21" sheetId="75" r:id="rId6"/>
+    <x:sheet name="12-13-21" sheetId="14" r:id="rId14"/>
+    <x:sheet name="12-20-21" sheetId="15" r:id="rId15"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Dummy Schedule - Dec 6'!$B$44:$C$86</x:definedName>
+    <x:definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'12-6-21'!$B$44:$C$86</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="191028"/>
   <x:extLst>
@@ -796,55 +797,124 @@
     <x:t>*REMINDER: schedule showcases when we do QC for Week 6!</x:t>
   </x:si>
   <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
     <x:t>Oct4 ServiceNow</x:t>
   </x:si>
   <x:si>
+    <x:t>30</x:t>
+  </x:si>
+  <x:si>
     <x:t>cumulative</x:t>
   </x:si>
   <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
     <x:t>Oct25 Java/React Enterprise</x:t>
   </x:si>
   <x:si>
+    <x:t>26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
     <x:t>Oct11 Java Extended</x:t>
   </x:si>
   <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
     <x:t>Nov01 Java/React Enterprise</x:t>
   </x:si>
   <x:si>
+    <x:t>28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
     <x:t>Dec 6 .NET Extended</x:t>
   </x:si>
   <x:si>
     <x:t>Reston</x:t>
   </x:si>
   <x:si>
+    <x:t>7</x:t>
+  </x:si>
+  <x:si>
     <x:t>Nov29 Java Angular/Enterprise</x:t>
   </x:si>
   <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
     <x:t>Oct25 Mulesoft</x:t>
   </x:si>
   <x:si>
+    <x:t>9</x:t>
+  </x:si>
+  <x:si>
     <x:t>Sept27 Java</x:t>
   </x:si>
   <x:si>
+    <x:t>25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10</x:t>
+  </x:si>
+  <x:si>
     <x:t>Sept27 UiPath</x:t>
   </x:si>
   <x:si>
+    <x:t>11</x:t>
+  </x:si>
+  <x:si>
     <x:t>Oct4 Big Data</x:t>
   </x:si>
   <x:si>
+    <x:t>29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12</x:t>
+  </x:si>
+  <x:si>
     <x:t>Oct4 .NET Extended</x:t>
   </x:si>
   <x:si>
+    <x:t>27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13</x:t>
+  </x:si>
+  <x:si>
     <x:t>Oct11 Big Data</x:t>
   </x:si>
   <x:si>
+    <x:t>17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15</x:t>
+  </x:si>
+  <x:si>
     <x:t>Oct11 Salesforce</x:t>
   </x:si>
   <x:si>
     <x:t>Tue</x:t>
   </x:si>
   <x:si>
-    <x:t>12</x:t>
+    <x:t>16</x:t>
   </x:si>
   <x:si>
     <x:t>Nov08 Salesforce</x:t>
@@ -853,12 +923,21 @@
     <x:t>Nov01 Java / React Extended</x:t>
   </x:si>
   <x:si>
+    <x:t>18</x:t>
+  </x:si>
+  <x:si>
     <x:t xml:space="preserve">Nov 15 Salesforce </x:t>
   </x:si>
   <x:si>
+    <x:t>19</x:t>
+  </x:si>
+  <x:si>
     <x:t>Dec 6 Salesforce</x:t>
   </x:si>
   <x:si>
+    <x:t>20</x:t>
+  </x:si>
+  <x:si>
     <x:t>Dec 6 Java Extended</x:t>
   </x:si>
   <x:si>
@@ -868,12 +947,27 @@
     <x:t xml:space="preserve"> </x:t>
   </x:si>
   <x:si>
+    <x:t>21</x:t>
+  </x:si>
+  <x:si>
     <x:t>Nov29 Big Data - Scala/Spark</x:t>
   </x:si>
   <x:si>
+    <x:t>0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22</x:t>
+  </x:si>
+  <x:si>
     <x:t>Nov29 Java Extended</x:t>
   </x:si>
   <x:si>
+    <x:t>32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23</x:t>
+  </x:si>
+  <x:si>
     <x:t>Nov 15 Java/Python w/Automation</x:t>
   </x:si>
   <x:si>
@@ -883,9 +977,15 @@
     <x:t>ET (Eastern Time)</x:t>
   </x:si>
   <x:si>
+    <x:t>24</x:t>
+  </x:si>
+  <x:si>
     <x:t>Sept13 Java Extended</x:t>
   </x:si>
   <x:si>
+    <x:t>34</x:t>
+  </x:si>
+  <x:si>
     <x:t>Oct18 JwA Extended</x:t>
   </x:si>
   <x:si>
@@ -901,6 +1001,9 @@
     <x:t>Nov 15 JwA Extended</x:t>
   </x:si>
   <x:si>
+    <x:t>31</x:t>
+  </x:si>
+  <x:si>
     <x:t>Dec 6 DynamicsCRM</x:t>
   </x:si>
   <x:si>
@@ -941,108 +1044,6 @@
   </x:si>
   <x:si>
     <x:t>AVAILABLE?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29</x:t>
-  </x:si>
-  <x:si>
-    <x:t>27</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>22</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23</x:t>
-  </x:si>
-  <x:si>
-    <x:t>24</x:t>
-  </x:si>
-  <x:si>
-    <x:t>34</x:t>
-  </x:si>
-  <x:si>
-    <x:t>31</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -3940,8 +3941,8 @@
   </x:sheetPr>
   <x:dimension ref="A1:O981"/>
   <x:sheetViews>
-    <x:sheetView topLeftCell="A30" workbookViewId="0">
-      <x:selection activeCell="I3" sqref="I3 I3:I35"/>
+    <x:sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <x:selection activeCell="I8" sqref="I8"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="255" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4025,20 +4026,20 @@
       <x:c r="M2" s="7" t="s"/>
     </x:row>
     <x:row r="3" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="10" t="n">
-        <x:v>2</x:v>
+      <x:c r="A3" s="10" t="s">
+        <x:v>251</x:v>
       </x:c>
       <x:c r="B3" s="4" t="s">
-        <x:v>251</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="C3" s="4" t="s">
         <x:v>76</x:v>
       </x:c>
-      <x:c r="D3" s="9" t="n">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="E3" s="9" t="n">
-        <x:v>2</x:v>
+      <x:c r="D3" s="9" t="s">
+        <x:v>253</x:v>
+      </x:c>
+      <x:c r="E3" s="9" t="s">
+        <x:v>251</x:v>
       </x:c>
       <x:c r="F3" s="9">
         <x:f>D3*E3</x:f>
@@ -4053,24 +4054,24 @@
       <x:c r="K3" s="30" t="s"/>
       <x:c r="L3" s="0" t="s"/>
       <x:c r="M3" s="31" t="s">
-        <x:v>252</x:v>
+        <x:v>254</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="10" t="n">
-        <x:v>3</x:v>
+      <x:c r="A4" s="10" t="s">
+        <x:v>255</x:v>
       </x:c>
       <x:c r="B4" s="4" t="s">
-        <x:v>253</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C4" s="4" t="s">
         <x:v>62</x:v>
       </x:c>
-      <x:c r="D4" s="9" t="n">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="E4" s="9" t="n">
-        <x:v>1.5</x:v>
+      <x:c r="D4" s="9" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="E4" s="9" t="s">
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F4" s="9">
         <x:f>D4*E4</x:f>
@@ -4087,20 +4088,20 @@
       <x:c r="M4" s="31" t="s"/>
     </x:row>
     <x:row r="5" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="10" t="n">
-        <x:v>4</x:v>
+      <x:c r="A5" s="10" t="s">
+        <x:v>259</x:v>
       </x:c>
       <x:c r="B5" s="4" t="s">
-        <x:v>254</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C5" s="4" t="s">
         <x:v>130</x:v>
       </x:c>
-      <x:c r="D5" s="9" t="n">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="E5" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D5" s="9" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="E5" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F5" s="9">
         <x:f>D5*E5</x:f>
@@ -4117,20 +4118,20 @@
       <x:c r="M5" s="31" t="s"/>
     </x:row>
     <x:row r="6" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="10" t="n">
-        <x:v>5</x:v>
+      <x:c r="A6" s="10" t="s">
+        <x:v>262</x:v>
       </x:c>
       <x:c r="B6" s="4" t="s">
-        <x:v>255</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="C6" s="4" t="s">
         <x:v>80</x:v>
       </x:c>
-      <x:c r="D6" s="9" t="n">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E6" s="9" t="n">
-        <x:v>1.5</x:v>
+      <x:c r="D6" s="9" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E6" s="9" t="s">
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F6" s="9">
         <x:f>D6*E6</x:f>
@@ -4147,20 +4148,20 @@
       <x:c r="M6" s="31" t="s"/>
     </x:row>
     <x:row r="7" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="10" t="n">
-        <x:v>6</x:v>
+      <x:c r="A7" s="10" t="s">
+        <x:v>265</x:v>
       </x:c>
       <x:c r="B7" s="4" t="s">
-        <x:v>256</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="C7" s="4" t="s">
         <x:v>141</x:v>
       </x:c>
-      <x:c r="D7" s="9" t="n">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="E7" s="9" t="n">
-        <x:v>1.5</x:v>
+      <x:c r="D7" s="9" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="E7" s="9" t="s">
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F7" s="9">
         <x:f>D7*E7</x:f>
@@ -4180,7 +4181,7 @@
     </x:row>
     <x:row r="8" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A8" s="8" t="s">
-        <x:v>257</x:v>
+        <x:v>267</x:v>
       </x:c>
       <x:c r="B8" s="4" t="s"/>
       <x:c r="C8" s="4" t="s"/>
@@ -4194,20 +4195,20 @@
       <x:c r="M8" s="31" t="s"/>
     </x:row>
     <x:row r="9" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="10" t="n">
-        <x:v>7</x:v>
+      <x:c r="A9" s="10" t="s">
+        <x:v>268</x:v>
       </x:c>
       <x:c r="B9" s="4" t="s">
-        <x:v>258</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="C9" s="4" t="s">
         <x:v>91</x:v>
       </x:c>
-      <x:c r="D9" s="9" t="n">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E9" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D9" s="9" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E9" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F9" s="9">
         <x:f>D9*E9</x:f>
@@ -4223,20 +4224,20 @@
       <x:c r="M9" s="31" t="s"/>
     </x:row>
     <x:row r="10" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A10" s="10" t="n">
-        <x:v>8</x:v>
+      <x:c r="A10" s="10" t="s">
+        <x:v>270</x:v>
       </x:c>
       <x:c r="B10" s="4" t="s">
-        <x:v>259</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="C10" s="4" t="s">
         <x:v>100</x:v>
       </x:c>
-      <x:c r="D10" s="9" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E10" s="9" t="n">
-        <x:v>2</x:v>
+      <x:c r="D10" s="9" t="s">
+        <x:v>270</x:v>
+      </x:c>
+      <x:c r="E10" s="9" t="s">
+        <x:v>251</x:v>
       </x:c>
       <x:c r="F10" s="9">
         <x:f>D10*E10</x:f>
@@ -4252,20 +4253,20 @@
       <x:c r="M10" s="31" t="s"/>
     </x:row>
     <x:row r="11" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="10" t="n">
-        <x:v>9</x:v>
+      <x:c r="A11" s="10" t="s">
+        <x:v>272</x:v>
       </x:c>
       <x:c r="B11" s="4" t="s">
-        <x:v>260</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="C11" s="4" t="s">
         <x:v>108</x:v>
       </x:c>
-      <x:c r="D11" s="9" t="n">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="E11" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D11" s="9" t="s">
+        <x:v>274</x:v>
+      </x:c>
+      <x:c r="E11" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F11" s="9">
         <x:f>D11*E11</x:f>
@@ -4284,20 +4285,20 @@
       </x:c>
     </x:row>
     <x:row r="12" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A12" s="10" t="n">
-        <x:v>10</x:v>
+      <x:c r="A12" s="10" t="s">
+        <x:v>275</x:v>
       </x:c>
       <x:c r="B12" s="4" t="s">
-        <x:v>261</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="C12" s="4" t="s">
         <x:v>112</x:v>
       </x:c>
-      <x:c r="D12" s="9" t="n">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="E12" s="9" t="n">
-        <x:v>2</x:v>
+      <x:c r="D12" s="9" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="E12" s="9" t="s">
+        <x:v>251</x:v>
       </x:c>
       <x:c r="F12" s="9">
         <x:f>D12*E12</x:f>
@@ -4316,20 +4317,20 @@
       </x:c>
     </x:row>
     <x:row r="13" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A13" s="10" t="n">
-        <x:v>11</x:v>
+      <x:c r="A13" s="10" t="s">
+        <x:v>277</x:v>
       </x:c>
       <x:c r="B13" s="4" t="s">
-        <x:v>262</x:v>
+        <x:v>278</x:v>
       </x:c>
       <x:c r="C13" s="4" t="s">
         <x:v>119</x:v>
       </x:c>
-      <x:c r="D13" s="9" t="n">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E13" s="9" t="n">
-        <x:v>2</x:v>
+      <x:c r="D13" s="9" t="s">
+        <x:v>279</x:v>
+      </x:c>
+      <x:c r="E13" s="9" t="s">
+        <x:v>251</x:v>
       </x:c>
       <x:c r="F13" s="9">
         <x:f>D13*E13</x:f>
@@ -4346,20 +4347,20 @@
       <x:c r="M13" s="31" t="s"/>
     </x:row>
     <x:row r="14" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A14" s="10" t="n">
-        <x:v>12</x:v>
+      <x:c r="A14" s="10" t="s">
+        <x:v>280</x:v>
       </x:c>
       <x:c r="B14" s="4" t="s">
-        <x:v>263</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="C14" s="4" t="s">
         <x:v>124</x:v>
       </x:c>
-      <x:c r="D14" s="9" t="n">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="E14" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D14" s="9" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="E14" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F14" s="9">
         <x:f>D14*E14</x:f>
@@ -4376,20 +4377,20 @@
       <x:c r="M14" s="31" t="s"/>
     </x:row>
     <x:row r="15" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A15" s="10" t="n">
-        <x:v>13</x:v>
+      <x:c r="A15" s="10" t="s">
+        <x:v>283</x:v>
       </x:c>
       <x:c r="B15" s="4" t="s">
-        <x:v>264</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="C15" s="4" t="s">
         <x:v>107</x:v>
       </x:c>
-      <x:c r="D15" s="9" t="n">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E15" s="9" t="n">
-        <x:v>1.5</x:v>
+      <x:c r="D15" s="9" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="E15" s="9" t="s">
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F15" s="9">
         <x:f>D15*E15</x:f>
@@ -4406,20 +4407,20 @@
       <x:c r="M15" s="31" t="s"/>
     </x:row>
     <x:row r="16" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A16" s="10" t="n">
-        <x:v>14</x:v>
+      <x:c r="A16" s="10" t="s">
+        <x:v>286</x:v>
       </x:c>
       <x:c r="B16" s="4" t="s">
-        <x:v>254</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C16" s="4" t="s">
         <x:v>127</x:v>
       </x:c>
-      <x:c r="D16" s="9" t="n">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E16" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D16" s="9" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E16" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F16" s="9">
         <x:f>D16*E16</x:f>
@@ -4436,20 +4437,20 @@
       <x:c r="M16" s="31" t="s"/>
     </x:row>
     <x:row r="17" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A17" s="10" t="n">
-        <x:v>15</x:v>
+      <x:c r="A17" s="10" t="s">
+        <x:v>287</x:v>
       </x:c>
       <x:c r="B17" s="4" t="s">
-        <x:v>265</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="C17" s="4" t="s">
         <x:v>129</x:v>
       </x:c>
-      <x:c r="D17" s="9" t="n">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="E17" s="9" t="n">
-        <x:v>1.5</x:v>
+      <x:c r="D17" s="9" t="s">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="E17" s="9" t="s">
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F17" s="9">
         <x:f>D17*E17</x:f>
@@ -4462,31 +4463,31 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="J17" s="0" t="s">
-        <x:v>266</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="K17" s="30">
         <x:v>0.416666666666667</x:v>
       </x:c>
       <x:c r="L17" s="11" t="s">
-        <x:v>267</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="M17" s="31" t="s"/>
     </x:row>
     <x:row r="18" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A18" s="10" t="n">
-        <x:v>16</x:v>
+      <x:c r="A18" s="10" t="s">
+        <x:v>290</x:v>
       </x:c>
       <x:c r="B18" s="4" t="s">
-        <x:v>268</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="C18" s="4" t="s">
         <x:v>131</x:v>
       </x:c>
-      <x:c r="D18" s="9" t="n">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E18" s="9" t="n">
-        <x:v>1.5</x:v>
+      <x:c r="D18" s="9" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E18" s="9" t="s">
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F18" s="9">
         <x:f>D18*E18</x:f>
@@ -4499,31 +4500,31 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="J18" s="0" t="s">
-        <x:v>266</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="K18" s="30">
         <x:v>0.416666666666667</x:v>
       </x:c>
       <x:c r="L18" s="11" t="s">
-        <x:v>267</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="M18" s="31" t="s"/>
     </x:row>
     <x:row r="19" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A19" s="10" t="n">
-        <x:v>17</x:v>
+      <x:c r="A19" s="10" t="s">
+        <x:v>285</x:v>
       </x:c>
       <x:c r="B19" s="4" t="s">
-        <x:v>269</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="C19" s="4" t="s">
         <x:v>133</x:v>
       </x:c>
-      <x:c r="D19" s="9" t="n">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E19" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D19" s="9" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E19" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F19" s="9">
         <x:f>D19*E19</x:f>
@@ -4540,20 +4541,20 @@
       <x:c r="M19" s="31" t="s"/>
     </x:row>
     <x:row r="20" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A20" s="10" t="n">
-        <x:v>18</x:v>
+      <x:c r="A20" s="10" t="s">
+        <x:v>293</x:v>
       </x:c>
       <x:c r="B20" s="4" t="s">
-        <x:v>270</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="C20" s="4" t="s">
         <x:v>134</x:v>
       </x:c>
-      <x:c r="D20" s="9" t="n">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E20" s="9" t="n">
-        <x:v>1.5</x:v>
+      <x:c r="D20" s="9" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E20" s="9" t="s">
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F20" s="9">
         <x:f>D20*E20</x:f>
@@ -4566,31 +4567,31 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="J20" s="0" t="s">
-        <x:v>266</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="K20" s="30">
         <x:v>0.416666666666667</x:v>
       </x:c>
       <x:c r="L20" s="11" t="s">
-        <x:v>267</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="M20" s="31" t="s"/>
     </x:row>
     <x:row r="21" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A21" s="10" t="n">
-        <x:v>19</x:v>
+      <x:c r="A21" s="10" t="s">
+        <x:v>295</x:v>
       </x:c>
       <x:c r="B21" s="4" t="s">
-        <x:v>271</x:v>
+        <x:v>296</x:v>
       </x:c>
       <x:c r="C21" s="4" t="s">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="D21" s="9" t="n">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="E21" s="9" t="n">
-        <x:v>1.5</x:v>
+      <x:c r="D21" s="9" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="E21" s="9" t="s">
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F21" s="9">
         <x:f>D21*E21</x:f>
@@ -4609,20 +4610,20 @@
       </x:c>
     </x:row>
     <x:row r="22" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A22" s="10" t="n">
-        <x:v>20</x:v>
+      <x:c r="A22" s="10" t="s">
+        <x:v>297</x:v>
       </x:c>
       <x:c r="B22" s="4" t="s">
-        <x:v>272</x:v>
+        <x:v>298</x:v>
       </x:c>
       <x:c r="C22" s="4" t="s">
         <x:v>136</x:v>
       </x:c>
-      <x:c r="D22" s="9" t="n">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E22" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D22" s="9" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E22" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F22" s="9">
         <x:f>D22*E22</x:f>
@@ -4642,7 +4643,7 @@
     </x:row>
     <x:row r="23" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A23" s="8" t="s">
-        <x:v>273</x:v>
+        <x:v>299</x:v>
       </x:c>
       <x:c r="B23" s="4" t="s"/>
       <x:c r="C23" s="4" t="s"/>
@@ -4650,7 +4651,7 @@
       <x:c r="E23" s="9" t="s"/>
       <x:c r="F23" s="9" t="s"/>
       <x:c r="G23" s="4" t="s">
-        <x:v>274</x:v>
+        <x:v>300</x:v>
       </x:c>
       <x:c r="H23" s="4" t="s"/>
       <x:c r="I23" s="9" t="s"/>
@@ -4658,20 +4659,20 @@
       <x:c r="M23" s="31" t="s"/>
     </x:row>
     <x:row r="24" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A24" s="10" t="n">
-        <x:v>21</x:v>
+      <x:c r="A24" s="10" t="s">
+        <x:v>301</x:v>
       </x:c>
       <x:c r="B24" s="4" t="s">
-        <x:v>275</x:v>
+        <x:v>302</x:v>
       </x:c>
       <x:c r="C24" s="4" t="s">
         <x:v>138</x:v>
       </x:c>
-      <x:c r="D24" s="9" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E24" s="9" t="n">
-        <x:v>1.5</x:v>
+      <x:c r="D24" s="9" t="s">
+        <x:v>303</x:v>
+      </x:c>
+      <x:c r="E24" s="9" t="s">
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F24" s="9">
         <x:f>D24*E24</x:f>
@@ -4687,20 +4688,20 @@
       <x:c r="M24" s="31" t="s"/>
     </x:row>
     <x:row r="25" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A25" s="10" t="n">
-        <x:v>22</x:v>
+      <x:c r="A25" s="10" t="s">
+        <x:v>304</x:v>
       </x:c>
       <x:c r="B25" s="4" t="s">
-        <x:v>276</x:v>
+        <x:v>305</x:v>
       </x:c>
       <x:c r="C25" s="4" t="s">
         <x:v>140</x:v>
       </x:c>
-      <x:c r="D25" s="9" t="n">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="E25" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D25" s="9" t="s">
+        <x:v>306</x:v>
+      </x:c>
+      <x:c r="E25" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F25" s="9">
         <x:f>D25*E25</x:f>
@@ -4716,20 +4717,20 @@
       <x:c r="M25" s="31" t="s"/>
     </x:row>
     <x:row r="26" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A26" s="10" t="n">
-        <x:v>23</x:v>
+      <x:c r="A26" s="10" t="s">
+        <x:v>307</x:v>
       </x:c>
       <x:c r="B26" s="4" t="s">
-        <x:v>277</x:v>
+        <x:v>308</x:v>
       </x:c>
       <x:c r="C26" s="4" t="s">
         <x:v>143</x:v>
       </x:c>
-      <x:c r="D26" s="9" t="n">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E26" s="9" t="n">
-        <x:v>1.5</x:v>
+      <x:c r="D26" s="9" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E26" s="9" t="s">
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F26" s="9">
         <x:f>D26*E26</x:f>
@@ -4747,10 +4748,10 @@
     </x:row>
     <x:row r="27" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A27" s="8" t="s">
-        <x:v>278</x:v>
+        <x:v>309</x:v>
       </x:c>
       <x:c r="B27" s="3" t="s">
-        <x:v>279</x:v>
+        <x:v>310</x:v>
       </x:c>
       <x:c r="C27" s="4" t="s"/>
       <x:c r="D27" s="9" t="s"/>
@@ -4763,20 +4764,20 @@
       <x:c r="M27" s="31" t="s"/>
     </x:row>
     <x:row r="28" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A28" s="10" t="n">
-        <x:v>24</x:v>
+      <x:c r="A28" s="10" t="s">
+        <x:v>311</x:v>
       </x:c>
       <x:c r="B28" s="16" t="s">
-        <x:v>280</x:v>
+        <x:v>312</x:v>
       </x:c>
       <x:c r="C28" s="4" t="s">
         <x:v>144</x:v>
       </x:c>
-      <x:c r="D28" s="9" t="n">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="E28" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D28" s="9" t="s">
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="E28" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F28" s="9">
         <x:f>D28*E28</x:f>
@@ -4795,20 +4796,20 @@
       </x:c>
     </x:row>
     <x:row r="29" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A29" s="10" t="n">
-        <x:v>25</x:v>
+      <x:c r="A29" s="10" t="s">
+        <x:v>274</x:v>
       </x:c>
       <x:c r="B29" s="16" t="s">
-        <x:v>254</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C29" s="4" t="s">
         <x:v>82</x:v>
       </x:c>
-      <x:c r="D29" s="9" t="n">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E29" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D29" s="9" t="s">
+        <x:v>279</x:v>
+      </x:c>
+      <x:c r="E29" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F29" s="9">
         <x:f>D29*E29</x:f>
@@ -4826,20 +4827,20 @@
       <x:c r="M29" s="31" t="s"/>
     </x:row>
     <x:row r="30" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A30" s="10" t="n">
-        <x:v>26</x:v>
+      <x:c r="A30" s="10" t="s">
+        <x:v>257</x:v>
       </x:c>
       <x:c r="B30" s="16" t="s">
-        <x:v>281</x:v>
+        <x:v>314</x:v>
       </x:c>
       <x:c r="C30" s="4" t="s">
         <x:v>145</x:v>
       </x:c>
-      <x:c r="D30" s="9" t="n">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="E30" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D30" s="9" t="s">
+        <x:v>306</x:v>
+      </x:c>
+      <x:c r="E30" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F30" s="9">
         <x:f>D30*E30</x:f>
@@ -4856,20 +4857,20 @@
       <x:c r="M30" s="31" t="s"/>
     </x:row>
     <x:row r="31" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A31" s="10" t="n">
-        <x:v>27</x:v>
+      <x:c r="A31" s="10" t="s">
+        <x:v>282</x:v>
       </x:c>
       <x:c r="B31" s="16" t="s">
-        <x:v>282</x:v>
+        <x:v>315</x:v>
       </x:c>
       <x:c r="C31" s="4" t="s">
         <x:v>120</x:v>
       </x:c>
-      <x:c r="D31" s="9" t="n">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="E31" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D31" s="9" t="s">
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="E31" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F31" s="9">
         <x:f>D31*E31</x:f>
@@ -4886,20 +4887,20 @@
       <x:c r="M31" s="31" t="s"/>
     </x:row>
     <x:row r="32" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A32" s="10" t="n">
-        <x:v>28</x:v>
+      <x:c r="A32" s="10" t="s">
+        <x:v>264</x:v>
       </x:c>
       <x:c r="B32" s="16" t="s">
-        <x:v>283</x:v>
+        <x:v>316</x:v>
       </x:c>
       <x:c r="C32" s="4" t="s">
         <x:v>146</x:v>
       </x:c>
-      <x:c r="D32" s="9" t="n">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="E32" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D32" s="9" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="E32" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F32" s="9">
         <x:f>D32*E32</x:f>
@@ -4916,20 +4917,20 @@
       <x:c r="M32" s="31" t="s"/>
     </x:row>
     <x:row r="33" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A33" s="10" t="n">
-        <x:v>29</x:v>
+      <x:c r="A33" s="10" t="s">
+        <x:v>279</x:v>
       </x:c>
       <x:c r="B33" s="16" t="s">
-        <x:v>284</x:v>
+        <x:v>317</x:v>
       </x:c>
       <x:c r="C33" s="4" t="s">
         <x:v>148</x:v>
       </x:c>
-      <x:c r="D33" s="9" t="n">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E33" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D33" s="9" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E33" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F33" s="9">
         <x:f>D33*E33</x:f>
@@ -4946,20 +4947,20 @@
       <x:c r="M33" s="31" t="s"/>
     </x:row>
     <x:row r="34" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A34" s="10" t="n">
-        <x:v>30</x:v>
+      <x:c r="A34" s="10" t="s">
+        <x:v>253</x:v>
       </x:c>
       <x:c r="B34" s="16" t="s">
-        <x:v>285</x:v>
+        <x:v>318</x:v>
       </x:c>
       <x:c r="C34" s="4" t="s">
         <x:v>147</x:v>
       </x:c>
-      <x:c r="D34" s="9" t="n">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E34" s="9" t="n">
-        <x:v>1</x:v>
+      <x:c r="D34" s="9" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E34" s="9" t="s">
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F34" s="9">
         <x:f>D34*E34</x:f>
@@ -4976,20 +4977,20 @@
       <x:c r="M34" s="31" t="s"/>
     </x:row>
     <x:row r="35" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A35" s="10" t="n">
-        <x:v>31</x:v>
+      <x:c r="A35" s="10" t="s">
+        <x:v>319</x:v>
       </x:c>
       <x:c r="B35" s="16" t="s">
-        <x:v>286</x:v>
+        <x:v>320</x:v>
       </x:c>
       <x:c r="C35" s="4" t="s">
         <x:v>149</x:v>
       </x:c>
-      <x:c r="D35" s="9" t="n">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="E35" s="9" t="n">
-        <x:v>1.5</x:v>
+      <x:c r="D35" s="9" t="s">
+        <x:v>304</x:v>
+      </x:c>
+      <x:c r="E35" s="9" t="s">
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F35" s="9">
         <x:f>D35*E35</x:f>
@@ -5010,17 +5011,17 @@
     <x:row r="36" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B36" s="4" t="s"/>
       <x:c r="C36" s="137" t="s">
-        <x:v>287</x:v>
+        <x:v>321</x:v>
       </x:c>
       <x:c r="D36" s="138" t="s"/>
       <x:c r="E36" s="139" t="s">
-        <x:v>288</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="F36" s="140" t="s">
-        <x:v>289</x:v>
+        <x:v>323</x:v>
       </x:c>
       <x:c r="G36" s="140" t="s">
-        <x:v>290</x:v>
+        <x:v>324</x:v>
       </x:c>
       <x:c r="K36" s="14" t="s"/>
       <x:c r="L36" s="15" t="s"/>
@@ -5028,7 +5029,7 @@
     </x:row>
     <x:row r="37" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B37" s="14" t="s">
-        <x:v>291</x:v>
+        <x:v>325</x:v>
       </x:c>
       <x:c r="C37" s="141" t="s">
         <x:v>35</x:v>
@@ -5075,7 +5076,7 @@
     <x:row r="39" spans="1:15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A39" s="10" t="s"/>
       <x:c r="B39" s="14" t="s">
-        <x:v>292</x:v>
+        <x:v>326</x:v>
       </x:c>
       <x:c r="C39" s="141" t="s">
         <x:v>37</x:v>
@@ -5093,7 +5094,7 @@
         <x:f>SUMIF($G$3:$G$31, C39, $F$3:$F$31)</x:f>
       </x:c>
       <x:c r="J39" s="0" t="s">
-        <x:v>293</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="K39" s="14" t="s"/>
       <x:c r="L39" s="15" t="s"/>
@@ -5120,7 +5121,7 @@
         <x:f>SUMIF($G$3:$G$31, C40, $F$3:$F$31)</x:f>
       </x:c>
       <x:c r="J40" s="10" t="s">
-        <x:v>294</x:v>
+        <x:v>328</x:v>
       </x:c>
       <x:c r="L40" s="0" t="s"/>
       <x:c r="M40" s="7" t="s"/>
@@ -5144,7 +5145,7 @@
         <x:f>SUMIF($G$3:$G$31, C41, $F$3:$F$31)</x:f>
       </x:c>
       <x:c r="J41" s="0" t="s">
-        <x:v>295</x:v>
+        <x:v>329</x:v>
       </x:c>
       <x:c r="L41" s="0" t="s"/>
       <x:c r="M41" s="7" t="s"/>
@@ -5152,7 +5153,7 @@
     <x:row r="42" spans="1:15" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A42" s="10" t="s"/>
       <x:c r="C42" s="147" t="s">
-        <x:v>296</x:v>
+        <x:v>330</x:v>
       </x:c>
       <x:c r="D42" s="148">
         <x:f>SUM(D37:D40)</x:f>
@@ -5170,7 +5171,7 @@
     <x:row r="43" spans="1:15" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A43" s="10" t="s"/>
       <x:c r="C43" s="151" t="s">
-        <x:v>297</x:v>
+        <x:v>331</x:v>
       </x:c>
       <x:c r="D43" s="152">
         <x:f>D42/COUNTA(C37:C40)</x:f>
@@ -5188,10 +5189,10 @@
     <x:row r="44" spans="1:15" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A44" s="10" t="s"/>
       <x:c r="B44" s="155" t="s">
-        <x:v>298</x:v>
+        <x:v>332</x:v>
       </x:c>
       <x:c r="C44" s="156" t="s">
-        <x:v>299</x:v>
+        <x:v>333</x:v>
       </x:c>
       <x:c r="F44" s="9" t="s"/>
       <x:c r="L44" s="0" t="s"/>
@@ -13862,24 +13863,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0600-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:N37"/>
+  <x:dimension ref="A1:A1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <x:selection activeCell="I38" sqref="I38 I36:I38"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <x:cols>
-    <x:col min="1" max="1" width="9.109375" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="28.332031" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="18.441406" style="0" customWidth="1"/>
-  </x:cols>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:14">
       <x:c r="B1" s="0" t="s">
         <x:v>236</x:v>
       </x:c>
@@ -13920,7 +13914,7 @@
         <x:v>248</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:14">
       <x:c r="A2" s="0" t="s">
         <x:v>249</x:v>
       </x:c>
@@ -13928,726 +13922,1309 @@
         <x:v>250</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <x:row r="3" spans="1:14">
       <x:c r="A3" s="0" t="s">
-        <x:v>300</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
         <x:v>76</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>301</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>300</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="F3" s="0">
         <x:f>D3*E3</x:f>
       </x:c>
-      <x:c r="I3" s="0">
-        <x:f>9+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="4" spans="1:14">
       <x:c r="A4" s="0" t="s">
-        <x:v>302</x:v>
+        <x:v>255</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>253</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
         <x:v>62</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>303</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F4" s="0">
         <x:f>D4*E4</x:f>
       </x:c>
-      <x:c r="I4" s="0">
-        <x:f>6+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="5" spans="1:14">
       <x:c r="A5" s="0" t="s">
-        <x:v>305</x:v>
+        <x:v>259</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>254</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
         <x:v>130</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>303</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F5" s="0">
         <x:f>D5*E5</x:f>
       </x:c>
-      <x:c r="I5" s="0">
-        <x:f>8+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="6" spans="1:14">
       <x:c r="A6" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>255</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
         <x:v>80</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F6" s="0">
         <x:f>D6*E6</x:f>
       </x:c>
-      <x:c r="I6" s="0">
-        <x:f>5+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="7" spans="1:14">
       <x:c r="A7" s="0" t="s">
-        <x:v>309</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>256</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
         <x:v>141</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>303</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F7" s="0">
         <x:f>D7*E7</x:f>
       </x:c>
-      <x:c r="I7" s="0">
-        <x:f>0+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="8" spans="1:14">
       <x:c r="A8" s="0" t="s">
-        <x:v>257</x:v>
-      </x:c>
-      <x:c r="I8" s="0">
-        <x:f>+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <x:v>267</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:14">
       <x:c r="A9" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>258</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
         <x:v>91</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F9" s="0">
         <x:f>D9*E9</x:f>
       </x:c>
-      <x:c r="I9" s="0">
-        <x:f>1+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="10" spans="1:14">
       <x:c r="A10" s="0" t="s">
-        <x:v>311</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>259</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
         <x:v>100</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>311</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>300</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="F10" s="0">
         <x:f>D10*E10</x:f>
       </x:c>
-      <x:c r="I10" s="0">
-        <x:f>6+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="11" spans="1:14">
       <x:c r="A11" s="0" t="s">
-        <x:v>312</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>260</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
         <x:v>108</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>313</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F11" s="0">
         <x:f>D11*E11</x:f>
       </x:c>
-      <x:c r="I11" s="0">
-        <x:f>10+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="12" spans="1:14">
       <x:c r="A12" s="0" t="s">
-        <x:v>314</x:v>
+        <x:v>275</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>261</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
         <x:v>112</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>303</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>300</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="F12" s="0">
         <x:f>D12*E12</x:f>
       </x:c>
-      <x:c r="I12" s="0">
-        <x:f>10+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="13" spans="1:14">
       <x:c r="A13" s="0" t="s">
-        <x:v>315</x:v>
+        <x:v>277</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>262</x:v>
+        <x:v>278</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
         <x:v>119</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>316</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>300</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="F13" s="0">
         <x:f>D13*E13</x:f>
       </x:c>
-      <x:c r="I13" s="0">
-        <x:f>9+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="14" spans="1:14">
       <x:c r="A14" s="0" t="s">
-        <x:v>267</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>263</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
         <x:v>124</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>317</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F14" s="0">
         <x:f>D14*E14</x:f>
       </x:c>
-      <x:c r="I14" s="0">
-        <x:f>9+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="15" spans="1:14">
       <x:c r="A15" s="0" t="s">
-        <x:v>318</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>264</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
         <x:v>107</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>319</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F15" s="0">
         <x:f>D15*E15</x:f>
       </x:c>
-      <x:c r="I15" s="0">
-        <x:f>8+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="16" spans="1:14">
       <x:c r="A16" s="0" t="s">
-        <x:v>320</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>254</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
         <x:v>127</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F16" s="0">
         <x:f>D16*E16</x:f>
       </x:c>
-      <x:c r="I16" s="0">
-        <x:f>8+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="17" spans="1:14">
       <x:c r="A17" s="0" t="s">
-        <x:v>321</x:v>
+        <x:v>287</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>265</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
         <x:v>129</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>321</x:v>
+        <x:v>287</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F17" s="0">
         <x:f>D17*E17</x:f>
       </x:c>
-      <x:c r="I17" s="0">
-        <x:f>8+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="18" spans="1:14">
       <x:c r="A18" s="0" t="s">
-        <x:v>322</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>268</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
         <x:v>131</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F18" s="0">
         <x:f>D18*E18</x:f>
       </x:c>
-      <x:c r="I18" s="0">
-        <x:f>4+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="19" spans="1:14">
       <x:c r="A19" s="0" t="s">
-        <x:v>319</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>269</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
         <x:v>133</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F19" s="0">
         <x:f>D19*E19</x:f>
       </x:c>
-      <x:c r="I19" s="0">
-        <x:f>5+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="20" spans="1:14">
       <x:c r="A20" s="0" t="s">
-        <x:v>323</x:v>
+        <x:v>293</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>270</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
         <x:v>134</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F20" s="0">
         <x:f>D20*E20</x:f>
       </x:c>
-      <x:c r="I20" s="0">
-        <x:f>3+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="21" spans="1:14">
       <x:c r="A21" s="0" t="s">
-        <x:v>324</x:v>
+        <x:v>295</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>271</x:v>
+        <x:v>296</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
         <x:v>64</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>303</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F21" s="0">
         <x:f>D21*E21</x:f>
       </x:c>
-      <x:c r="I21" s="0">
-        <x:f>0+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="22" spans="1:14">
       <x:c r="A22" s="0" t="s">
-        <x:v>325</x:v>
+        <x:v>297</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>272</x:v>
+        <x:v>298</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
         <x:v>136</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F22" s="0">
         <x:f>D22*E22</x:f>
       </x:c>
-      <x:c r="I22" s="0">
-        <x:f>0+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="23" spans="1:14">
       <x:c r="A23" s="0" t="s">
-        <x:v>273</x:v>
-      </x:c>
-      <x:c r="I23" s="0">
-        <x:f>+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <x:v>299</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:14">
       <x:c r="A24" s="0" t="s">
-        <x:v>326</x:v>
+        <x:v>301</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>275</x:v>
+        <x:v>302</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
         <x:v>138</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>327</x:v>
+        <x:v>303</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F24" s="0">
         <x:f>D24*E24</x:f>
       </x:c>
-      <x:c r="I24" s="0">
-        <x:f>1+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="25" spans="1:14">
       <x:c r="A25" s="0" t="s">
-        <x:v>328</x:v>
+        <x:v>304</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>276</x:v>
+        <x:v>305</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
         <x:v>140</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>329</x:v>
+        <x:v>306</x:v>
       </x:c>
       <x:c r="E25" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F25" s="0">
         <x:f>D25*E25</x:f>
       </x:c>
-      <x:c r="I25" s="0">
-        <x:f>1+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="26" spans="1:14">
       <x:c r="A26" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>307</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>277</x:v>
+        <x:v>308</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
         <x:v>143</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F26" s="0">
         <x:f>D26*E26</x:f>
       </x:c>
-      <x:c r="I26" s="0">
-        <x:f>3+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="27" spans="1:14">
       <x:c r="A27" s="0" t="s">
-        <x:v>278</x:v>
+        <x:v>309</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>279</x:v>
-      </x:c>
-      <x:c r="I27" s="0">
-        <x:f>+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:14" x14ac:dyDescent="0.25">
+        <x:v>310</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:14">
       <x:c r="A28" s="0" t="s">
-        <x:v>331</x:v>
+        <x:v>311</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>280</x:v>
+        <x:v>312</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
         <x:v>144</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>332</x:v>
+        <x:v>313</x:v>
       </x:c>
       <x:c r="E28" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F28" s="0">
         <x:f>D28*E28</x:f>
       </x:c>
-      <x:c r="I28" s="0">
-        <x:f>12+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="29" spans="1:14">
       <x:c r="A29" s="0" t="s">
-        <x:v>313</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>254</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
         <x:v>82</x:v>
       </x:c>
       <x:c r="D29" s="0" t="s">
-        <x:v>316</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="E29" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F29" s="0">
         <x:f>D29*E29</x:f>
       </x:c>
-      <x:c r="I29" s="0">
-        <x:f>6+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="30" spans="1:14">
       <x:c r="A30" s="0" t="s">
-        <x:v>303</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>281</x:v>
+        <x:v>314</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
         <x:v>145</x:v>
       </x:c>
       <x:c r="D30" s="0" t="s">
-        <x:v>329</x:v>
+        <x:v>306</x:v>
       </x:c>
       <x:c r="E30" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F30" s="0">
         <x:f>D30*E30</x:f>
       </x:c>
-      <x:c r="I30" s="0">
-        <x:f>7+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="31" spans="1:14">
       <x:c r="A31" s="0" t="s">
-        <x:v>317</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>282</x:v>
+        <x:v>315</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
         <x:v>120</x:v>
       </x:c>
       <x:c r="D31" s="0" t="s">
-        <x:v>332</x:v>
+        <x:v>313</x:v>
       </x:c>
       <x:c r="E31" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F31" s="0">
         <x:f>D31*E31</x:f>
       </x:c>
-      <x:c r="I31" s="0">
-        <x:f>7+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="32" spans="1:14">
       <x:c r="A32" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>283</x:v>
+        <x:v>316</x:v>
       </x:c>
       <x:c r="C32" s="0" t="s">
         <x:v>146</x:v>
       </x:c>
       <x:c r="D32" s="0" t="s">
-        <x:v>317</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="E32" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F32" s="0">
         <x:f>D32*E32</x:f>
       </x:c>
-      <x:c r="I32" s="0">
-        <x:f>5+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="33" spans="1:14">
       <x:c r="A33" s="0" t="s">
-        <x:v>316</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>284</x:v>
+        <x:v>317</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
         <x:v>148</x:v>
       </x:c>
       <x:c r="D33" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E33" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F33" s="0">
         <x:f>D33*E33</x:f>
       </x:c>
-      <x:c r="I33" s="0">
-        <x:f>3+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="34" spans="1:14">
       <x:c r="A34" s="0" t="s">
-        <x:v>301</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>285</x:v>
+        <x:v>318</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
         <x:v>147</x:v>
       </x:c>
       <x:c r="D34" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E34" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F34" s="0">
         <x:f>D34*E34</x:f>
       </x:c>
-      <x:c r="I34" s="0">
-        <x:f>3+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    </x:row>
+    <x:row r="35" spans="1:14">
       <x:c r="A35" s="0" t="s">
-        <x:v>333</x:v>
+        <x:v>319</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>286</x:v>
+        <x:v>320</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
         <x:v>149</x:v>
       </x:c>
       <x:c r="D35" s="0" t="s">
-        <x:v>328</x:v>
+        <x:v>304</x:v>
       </x:c>
       <x:c r="E35" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F35" s="0">
         <x:f>D35*E35</x:f>
       </x:c>
-      <x:c r="I35" s="0">
-        <x:f>0+ 1</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <x:c r="F37" s="0">
-        <x:f>SUMIF($G$3:$G$34, C37, $D$3:$D$34)</x:f>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:14">
+      <x:c r="B1" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>237</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>238</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>239</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>240</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>241</x:v>
+      </x:c>
+      <x:c r="H1" s="0" t="s">
+        <x:v>242</x:v>
+      </x:c>
+      <x:c r="I1" s="0" t="s">
+        <x:v>243</x:v>
+      </x:c>
+      <x:c r="J1" s="0" t="s">
+        <x:v>244</x:v>
+      </x:c>
+      <x:c r="K1" s="0" t="s">
+        <x:v>245</x:v>
+      </x:c>
+      <x:c r="L1" s="0" t="s">
+        <x:v>246</x:v>
+      </x:c>
+      <x:c r="M1" s="0" t="s">
+        <x:v>247</x:v>
+      </x:c>
+      <x:c r="N1" s="0" t="s">
+        <x:v>248</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:14">
+      <x:c r="A2" s="0" t="s">
+        <x:v>249</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>250</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:14">
+      <x:c r="A3" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>252</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>253</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+      <x:c r="F3" s="0">
+        <x:f>D3*E3</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:14">
+      <x:c r="A4" s="0" t="s">
+        <x:v>255</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="F4" s="0">
+        <x:f>D4*E4</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:14">
+      <x:c r="A5" s="0" t="s">
+        <x:v>259</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F5" s="0">
+        <x:f>D5*E5</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:14">
+      <x:c r="A6" s="0" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>263</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="F6" s="0">
+        <x:f>D6*E6</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:14">
+      <x:c r="A7" s="0" t="s">
+        <x:v>265</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="F7" s="0">
+        <x:f>D7*E7</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:14">
+      <x:c r="A8" s="0" t="s">
+        <x:v>267</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:14">
+      <x:c r="A9" s="0" t="s">
+        <x:v>268</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>269</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F9" s="0">
+        <x:f>D9*E9</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:14">
+      <x:c r="A10" s="0" t="s">
+        <x:v>270</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>271</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>270</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+      <x:c r="F10" s="0">
+        <x:f>D10*E10</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:14">
+      <x:c r="A11" s="0" t="s">
+        <x:v>272</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>273</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>274</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F11" s="0">
+        <x:f>D11*E11</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:14">
+      <x:c r="A12" s="0" t="s">
+        <x:v>275</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>276</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+      <x:c r="F12" s="0">
+        <x:f>D12*E12</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:14">
+      <x:c r="A13" s="0" t="s">
+        <x:v>277</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>278</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>279</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+      <x:c r="F13" s="0">
+        <x:f>D13*E13</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:14">
+      <x:c r="A14" s="0" t="s">
+        <x:v>280</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>281</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F14" s="0">
+        <x:f>D14*E14</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:14">
+      <x:c r="A15" s="0" t="s">
+        <x:v>283</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>284</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="F15" s="0">
+        <x:f>D15*E15</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:14">
+      <x:c r="A16" s="0" t="s">
+        <x:v>286</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F16" s="0">
+        <x:f>D16*E16</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:14">
+      <x:c r="A17" s="0" t="s">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>288</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="F17" s="0">
+        <x:f>D17*E17</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:14">
+      <x:c r="A18" s="0" t="s">
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="F18" s="0">
+        <x:f>D18*E18</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:14">
+      <x:c r="A19" s="0" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F19" s="0">
+        <x:f>D19*E19</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:14">
+      <x:c r="A20" s="0" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>294</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="F20" s="0">
+        <x:f>D20*E20</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:14">
+      <x:c r="A21" s="0" t="s">
+        <x:v>295</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>296</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="F21" s="0">
+        <x:f>D21*E21</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:14">
+      <x:c r="A22" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>298</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F22" s="0">
+        <x:f>D22*E22</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:14">
+      <x:c r="A23" s="0" t="s">
+        <x:v>299</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:14">
+      <x:c r="A24" s="0" t="s">
+        <x:v>301</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>302</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>303</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="F24" s="0">
+        <x:f>D24*E24</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:14">
+      <x:c r="A25" s="0" t="s">
+        <x:v>304</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>306</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F25" s="0">
+        <x:f>D25*E25</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:14">
+      <x:c r="A26" s="0" t="s">
+        <x:v>307</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>308</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="F26" s="0">
+        <x:f>D26*E26</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:14">
+      <x:c r="A27" s="0" t="s">
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>310</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:14">
+      <x:c r="A28" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>312</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F28" s="0">
+        <x:f>D28*E28</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:14">
+      <x:c r="A29" s="0" t="s">
+        <x:v>274</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>279</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F29" s="0">
+        <x:f>D29*E29</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:14">
+      <x:c r="A30" s="0" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>314</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>306</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F30" s="0">
+        <x:f>D30*E30</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:14">
+      <x:c r="A31" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>315</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F31" s="0">
+        <x:f>D31*E31</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:14">
+      <x:c r="A32" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>316</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F32" s="0">
+        <x:f>D32*E32</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:14">
+      <x:c r="A33" s="0" t="s">
+        <x:v>279</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>317</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F33" s="0">
+        <x:f>D33*E33</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:14">
+      <x:c r="A34" s="0" t="s">
+        <x:v>253</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>318</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F34" s="0">
+        <x:f>D34*E34</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:14">
+      <x:c r="A35" s="0" t="s">
+        <x:v>319</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>149</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>304</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="F35" s="0">
+        <x:f>D35*E35</x:f>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -14660,6 +15237,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -14668,7 +15251,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010035320A12CFF460459638DE9B86DD9357" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f11676696cc246df58d12072c86cf252">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5789d6d3-4852-43c5-9082-41a0df76b368" xmlns:ns4="f28bebd9-3202-45a0-b989-5e5ae93a89b5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ea6d730d764c2aef8b02e40be4db643" ns3:_="" ns4:_="">
     <xsd:import namespace="5789d6d3-4852-43c5-9082-41a0df76b368"/>
@@ -14891,13 +15474,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B5B8A7-0BC9-4D7F-8134-9CC058C7B2A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18F62D5D-402C-4D37-8B1B-B293D3FE1710}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -14905,7 +15491,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E74CAD0-3F93-445C-B91B-678382B98543}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14922,13 +15508,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B5B8A7-0BC9-4D7F-8134-9CC058C7B2A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>